<commit_message>
Demand updated to annual values for initial years
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_Demand_BASE_UP.xlsx
+++ b/SuppXLS/Scen_Demand_BASE_UP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\GDrive\PhD\Veda_2\IrishTimes_GIT\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B26FE594-78E0-4030-B2B3-62856A220D2E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C7FB1F85-AF3C-42B5-9574-6A1C410376EB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
@@ -1126,7 +1126,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CL41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -5069,14 +5071,62 @@
       <c r="J17">
         <v>10.761291751557</v>
       </c>
+      <c r="K17">
+        <v>15.5599108867594</v>
+      </c>
+      <c r="L17">
+        <v>15.8733021678926</v>
+      </c>
+      <c r="M17">
+        <v>16.200818264161999</v>
+      </c>
+      <c r="N17">
+        <v>16.542462199289201</v>
+      </c>
       <c r="O17">
         <v>16.8982198327897</v>
       </c>
+      <c r="P17">
+        <v>17.268096881896099</v>
+      </c>
+      <c r="Q17">
+        <v>17.652033672042599</v>
+      </c>
+      <c r="R17">
+        <v>18.050103479220599</v>
+      </c>
+      <c r="S17">
+        <v>18.4623967755869</v>
+      </c>
       <c r="T17">
         <v>18.888828873499399</v>
       </c>
+      <c r="U17">
+        <v>19.289730524802501</v>
+      </c>
+      <c r="V17">
+        <v>19.704624475580701</v>
+      </c>
+      <c r="W17">
+        <v>20.133544789182899</v>
+      </c>
+      <c r="X17">
+        <v>20.576499533745501</v>
+      </c>
       <c r="Y17">
         <v>21.033406990161801</v>
+      </c>
+      <c r="Z17">
+        <v>21.504214270924201</v>
+      </c>
+      <c r="AA17">
+        <v>21.9888626351418</v>
+      </c>
+      <c r="AB17">
+        <v>22.4873044208891</v>
+      </c>
+      <c r="AC17">
+        <v>22.999440496836101</v>
       </c>
       <c r="AD17">
         <v>23.5251990234853</v>
@@ -5137,14 +5187,62 @@
       <c r="J18">
         <v>23.136777265847599</v>
       </c>
+      <c r="K18">
+        <v>33.453808406532801</v>
+      </c>
+      <c r="L18">
+        <v>34.127599660969103</v>
+      </c>
+      <c r="M18">
+        <v>34.8317592679483</v>
+      </c>
+      <c r="N18">
+        <v>35.566293728471699</v>
+      </c>
       <c r="O18">
         <v>36.331172640497797</v>
       </c>
+      <c r="P18">
+        <v>37.126408296076697</v>
+      </c>
+      <c r="Q18">
+        <v>37.951872394891602</v>
+      </c>
+      <c r="R18">
+        <v>38.807722480324202</v>
+      </c>
+      <c r="S18">
+        <v>39.694153067511799</v>
+      </c>
       <c r="T18">
         <v>40.610982078023703</v>
       </c>
+      <c r="U18">
+        <v>41.472920628325397</v>
+      </c>
+      <c r="V18">
+        <v>42.364942622498504</v>
+      </c>
+      <c r="W18">
+        <v>43.287121296743202</v>
+      </c>
+      <c r="X18">
+        <v>44.2394739975528</v>
+      </c>
       <c r="Y18">
         <v>45.221825028847903</v>
+      </c>
+      <c r="Z18">
+        <v>46.234060682486998</v>
+      </c>
+      <c r="AA18">
+        <v>47.276054665554803</v>
+      </c>
+      <c r="AB18">
+        <v>48.347704504911498</v>
+      </c>
+      <c r="AC18">
+        <v>49.448797068197599</v>
       </c>
       <c r="AD18">
         <v>50.579177900493498</v>
@@ -5205,14 +5303,62 @@
       <c r="J19">
         <v>19.9083897403805</v>
       </c>
+      <c r="K19">
+        <v>28.785835140505</v>
+      </c>
+      <c r="L19">
+        <v>29.3656090106013</v>
+      </c>
+      <c r="M19">
+        <v>29.971513788699699</v>
+      </c>
+      <c r="N19">
+        <v>30.603555068685001</v>
+      </c>
       <c r="O19">
         <v>31.261706690660901</v>
       </c>
+      <c r="P19">
+        <v>31.945979231507799</v>
+      </c>
+      <c r="Q19">
+        <v>32.6562622932788</v>
+      </c>
+      <c r="R19">
+        <v>33.392691436558003</v>
+      </c>
+      <c r="S19">
+        <v>34.1554340348357</v>
+      </c>
       <c r="T19">
         <v>34.944333415973901</v>
       </c>
+      <c r="U19">
+        <v>35.686001470884598</v>
+      </c>
+      <c r="V19">
+        <v>36.4535552798243</v>
+      </c>
+      <c r="W19">
+        <v>37.247057859988303</v>
+      </c>
+      <c r="X19">
+        <v>38.066524137429198</v>
+      </c>
       <c r="Y19">
         <v>38.911802931799301</v>
+      </c>
+      <c r="Z19">
+        <v>39.782796401209801</v>
+      </c>
+      <c r="AA19">
+        <v>40.679395875012297</v>
+      </c>
+      <c r="AB19">
+        <v>41.601513178644801</v>
+      </c>
+      <c r="AC19">
+        <v>42.548964919146698</v>
       </c>
       <c r="AD19">
         <v>43.5216181934479</v>
@@ -5265,13 +5411,40 @@
         <v>45</v>
       </c>
       <c r="H20">
-        <v>11.573</v>
+        <v>13.9338253594454</v>
+      </c>
+      <c r="I20">
+        <v>14.230644491946901</v>
       </c>
       <c r="J20">
         <v>11.754512350348101</v>
       </c>
+      <c r="K20">
+        <v>14.8433860204529</v>
+      </c>
+      <c r="L20">
+        <v>15.159580665377799</v>
+      </c>
+      <c r="M20">
+        <v>15.482510906435699</v>
+      </c>
+      <c r="N20">
+        <v>15.8123202256746</v>
+      </c>
       <c r="O20">
         <v>16.149155161605499</v>
+      </c>
+      <c r="P20">
+        <v>16.493165374310699</v>
+      </c>
+      <c r="Q20">
+        <v>16.844503711940099</v>
+      </c>
+      <c r="R20">
+        <v>17.203326278623699</v>
+      </c>
+      <c r="S20">
+        <v>17.569792503830101</v>
       </c>
       <c r="T20">
         <v>17.944065213203601</v>
@@ -6462,109 +6635,109 @@
         <v>57</v>
       </c>
       <c r="H26">
-        <v>213414.55695615499</v>
+        <v>213.414556956155</v>
       </c>
       <c r="I26">
-        <v>218956.66937259401</v>
+        <v>218.95666937259401</v>
       </c>
       <c r="J26">
-        <v>225300.33816185399</v>
+        <v>225.300338161854</v>
       </c>
       <c r="K26">
-        <v>242574.41637552099</v>
+        <v>242.574416375521</v>
       </c>
       <c r="L26">
-        <v>259561.94669652099</v>
+        <v>259.56194669652098</v>
       </c>
       <c r="M26">
-        <v>275023.94138045801</v>
+        <v>275.02394138045798</v>
       </c>
       <c r="N26">
-        <v>289113.78640676098</v>
+        <v>289.11378640676099</v>
       </c>
       <c r="O26">
-        <v>302217.18367944099</v>
+        <v>302.21718367944101</v>
       </c>
       <c r="P26">
-        <v>314549.61337722198</v>
+        <v>314.54961337722199</v>
       </c>
       <c r="Q26">
-        <v>326290.81316684798</v>
+        <v>326.29081316684801</v>
       </c>
       <c r="R26">
-        <v>337584.19698321301</v>
+        <v>337.58419698321302</v>
       </c>
       <c r="S26">
-        <v>348488.670477651</v>
+        <v>348.488670477651</v>
       </c>
       <c r="T26">
-        <v>359053.362495562</v>
+        <v>359.053362495562</v>
       </c>
       <c r="U26">
-        <v>379435.10129855498</v>
+        <v>379.43510129855503</v>
       </c>
       <c r="V26">
-        <v>394286.43020683102</v>
+        <v>394.28643020683103</v>
       </c>
       <c r="W26">
-        <v>409460.08200179902</v>
+        <v>409.46008200179898</v>
       </c>
       <c r="X26">
-        <v>424963.52313310798</v>
+        <v>424.96352313310803</v>
       </c>
       <c r="Y26">
-        <v>440776.66278306401</v>
+        <v>440.77666278306401</v>
       </c>
       <c r="Z26">
-        <v>456888.48985664902</v>
+        <v>456.88848985664902</v>
       </c>
       <c r="AA26">
-        <v>473286.23919771903</v>
+        <v>473.286239197719</v>
       </c>
       <c r="AB26">
-        <v>489960.78944409703</v>
+        <v>489.96078944409697</v>
       </c>
       <c r="AC26">
-        <v>506886.30914768699</v>
+        <v>506.88630914768697</v>
       </c>
       <c r="AD26">
-        <v>524045.59801496298</v>
+        <v>524.04559801496305</v>
       </c>
       <c r="AI26">
-        <v>632981.68201128603</v>
+        <v>632.98168201128601</v>
       </c>
       <c r="AN26">
-        <v>740749.97310115199</v>
+        <v>740.74997310115202</v>
       </c>
       <c r="AS26">
-        <v>853983.36761178297</v>
+        <v>853.983367611782</v>
       </c>
       <c r="AX26">
-        <v>973313.84240591305</v>
+        <v>973.31384240591296</v>
       </c>
       <c r="BC26">
-        <v>1101920.21948223</v>
+        <v>1101.9202194822301</v>
       </c>
       <c r="BH26">
-        <v>1243456.94226919</v>
+        <v>1243.45694226919</v>
       </c>
       <c r="BM26">
-        <v>1400399.1537987201</v>
+        <v>1400.3991537987199</v>
       </c>
       <c r="BR26">
-        <v>1574723.2584762699</v>
+        <v>1574.7232584762701</v>
       </c>
       <c r="BW26">
-        <v>1766492.4181818999</v>
+        <v>1766.4924181818999</v>
       </c>
       <c r="CB26">
-        <v>1974228.0679925601</v>
+        <v>1974.22806799256</v>
       </c>
       <c r="CG26">
-        <v>2195390.7432208802</v>
+        <v>2195.3907432208798</v>
       </c>
       <c r="CL26">
-        <v>2428365.4614147102</v>
+        <v>2428.3654614147099</v>
       </c>
     </row>
     <row r="27" spans="2:90" x14ac:dyDescent="0.25">
@@ -6578,109 +6751,109 @@
         <v>59</v>
       </c>
       <c r="H27">
-        <v>766617.95373000402</v>
+        <v>766.61795373000405</v>
       </c>
       <c r="I27">
-        <v>776019.61867223098</v>
+        <v>776.01961867223099</v>
       </c>
       <c r="J27">
-        <v>788300.85620074603</v>
+        <v>788.30085620074601</v>
       </c>
       <c r="K27">
-        <v>801957.14588082698</v>
+        <v>801.95714588082706</v>
       </c>
       <c r="L27">
-        <v>819060.32622000796</v>
+        <v>819.06032622000805</v>
       </c>
       <c r="M27">
-        <v>834661.58347222698</v>
+        <v>834.66158347222699</v>
       </c>
       <c r="N27">
-        <v>848818.67768832797</v>
+        <v>848.81867768832797</v>
       </c>
       <c r="O27">
-        <v>862331.35320143297</v>
+        <v>862.33135320143299</v>
       </c>
       <c r="P27">
-        <v>875509.45116964797</v>
+        <v>875.50945116964795</v>
       </c>
       <c r="Q27">
-        <v>888595.96249835705</v>
+        <v>888.59596249835704</v>
       </c>
       <c r="R27">
-        <v>901764.69015385106</v>
+        <v>901.76469015385101</v>
       </c>
       <c r="S27">
-        <v>914993.375655549</v>
+        <v>914.99337565554902</v>
       </c>
       <c r="T27">
-        <v>928266.37631273095</v>
+        <v>928.26637631273104</v>
       </c>
       <c r="U27">
-        <v>943708.89277841605</v>
+        <v>943.70889277841604</v>
       </c>
       <c r="V27">
-        <v>957570.71779714397</v>
+        <v>957.57071779714397</v>
       </c>
       <c r="W27">
-        <v>971442.33945732203</v>
+        <v>971.44233945732196</v>
       </c>
       <c r="X27">
-        <v>985334.55511306797</v>
+        <v>985.33455511306795</v>
       </c>
       <c r="Y27">
-        <v>999194.66131792602</v>
+        <v>999.19466131792603</v>
       </c>
       <c r="Z27">
-        <v>1012994.63657764</v>
+        <v>1012.99463657764</v>
       </c>
       <c r="AA27">
-        <v>1026705.03546086</v>
+        <v>1026.70503546086</v>
       </c>
       <c r="AB27">
-        <v>1040306.63185868</v>
+        <v>1040.30663185868</v>
       </c>
       <c r="AC27">
-        <v>1053747.0705237</v>
+        <v>1053.7470705236999</v>
       </c>
       <c r="AD27">
-        <v>1066995.89427272</v>
+        <v>1066.9958942727201</v>
       </c>
       <c r="AI27">
-        <v>1166763.43459146</v>
+        <v>1166.7634345914601</v>
       </c>
       <c r="AN27">
-        <v>1244336.6649656901</v>
+        <v>1244.33666496569</v>
       </c>
       <c r="AS27">
-        <v>1314710.96966167</v>
+        <v>1314.7109696616701</v>
       </c>
       <c r="AX27">
-        <v>1379878.79642933</v>
+        <v>1379.8787964293299</v>
       </c>
       <c r="BC27">
-        <v>1444629.9926038501</v>
+        <v>1444.62999260385</v>
       </c>
       <c r="BH27">
-        <v>1512989.3882673399</v>
+        <v>1512.98938826734</v>
       </c>
       <c r="BM27">
-        <v>1586512.86397531</v>
+        <v>1586.51286397531</v>
       </c>
       <c r="BR27">
-        <v>1665745.9920316101</v>
+        <v>1665.7459920316101</v>
       </c>
       <c r="BW27">
-        <v>1749111.94897432</v>
+        <v>1749.1119489743201</v>
       </c>
       <c r="CB27">
-        <v>1833896.3857972301</v>
+        <v>1833.8963857972301</v>
       </c>
       <c r="CG27">
-        <v>1917030.21036523</v>
+        <v>1917.03021036523</v>
       </c>
       <c r="CL27">
-        <v>1996868.66239624</v>
+        <v>1996.8686623962401</v>
       </c>
     </row>
     <row r="28" spans="2:90" x14ac:dyDescent="0.25">
@@ -6694,109 +6867,109 @@
         <v>61</v>
       </c>
       <c r="H28">
-        <v>721105.90866437601</v>
+        <v>721.10590866437599</v>
       </c>
       <c r="I28">
-        <v>729040.47594293603</v>
+        <v>729.04047594293604</v>
       </c>
       <c r="J28">
-        <v>739683.68570912001</v>
+        <v>739.68368570912003</v>
       </c>
       <c r="K28">
-        <v>748342.44886999705</v>
+        <v>748.34244886999704</v>
       </c>
       <c r="L28">
-        <v>760630.721289968</v>
+        <v>760.63072128996805</v>
       </c>
       <c r="M28">
-        <v>771850.38797134894</v>
+        <v>771.85038797134905</v>
       </c>
       <c r="N28">
-        <v>782013.10939486197</v>
+        <v>782.013109394862</v>
       </c>
       <c r="O28">
-        <v>791820.47563049395</v>
+        <v>791.820475630494</v>
       </c>
       <c r="P28">
-        <v>801523.77429367404</v>
+        <v>801.52377429367402</v>
       </c>
       <c r="Q28">
-        <v>811316.73568663199</v>
+        <v>811.316735686632</v>
       </c>
       <c r="R28">
-        <v>821333.312278467</v>
+        <v>821.33331227846702</v>
       </c>
       <c r="S28">
-        <v>831532.33535063395</v>
+        <v>831.53233535063396</v>
       </c>
       <c r="T28">
-        <v>841882.469887482</v>
+        <v>841.88246988748199</v>
       </c>
       <c r="U28">
-        <v>851415.47129100398</v>
+        <v>851.415471291004</v>
       </c>
       <c r="V28">
-        <v>861039.36197674705</v>
+        <v>861.03936197674705</v>
       </c>
       <c r="W28">
-        <v>870573.18258039001</v>
+        <v>870.57318258039004</v>
       </c>
       <c r="X28">
-        <v>880025.70362676098</v>
+        <v>880.02570362676101</v>
       </c>
       <c r="Y28">
-        <v>889349.03440936899</v>
+        <v>889.34903440936898</v>
       </c>
       <c r="Z28">
-        <v>898517.81453963905</v>
+        <v>898.51781453963895</v>
       </c>
       <c r="AA28">
-        <v>907505.76600673597</v>
+        <v>907.50576600673605</v>
       </c>
       <c r="AB28">
-        <v>916295.97516395</v>
+        <v>916.29597516394995</v>
       </c>
       <c r="AC28">
-        <v>924842.69231704494</v>
+        <v>924.84269231704502</v>
       </c>
       <c r="AD28">
-        <v>933119.97808990802</v>
+        <v>933.11997808990805</v>
       </c>
       <c r="AI28">
-        <v>1001750.03116784</v>
+        <v>1001.75003116784</v>
       </c>
       <c r="AN28">
-        <v>1047946.93470063</v>
+        <v>1047.94693470063</v>
       </c>
       <c r="AS28">
-        <v>1085051.9905217399</v>
+        <v>1085.05199052173</v>
       </c>
       <c r="AX28">
-        <v>1114915.32706986</v>
+        <v>1114.91532706986</v>
       </c>
       <c r="BC28">
-        <v>1141469.10325923</v>
+        <v>1141.46910325923</v>
       </c>
       <c r="BH28">
-        <v>1167711.9675762199</v>
+        <v>1167.7119675762201</v>
       </c>
       <c r="BM28">
-        <v>1194473.05229634</v>
+        <v>1194.47305229634</v>
       </c>
       <c r="BR28">
-        <v>1221698.7321783099</v>
+        <v>1221.6987321783099</v>
       </c>
       <c r="BW28">
-        <v>1247749.8188300601</v>
+        <v>1247.7498188300599</v>
       </c>
       <c r="CB28">
-        <v>1270297.7134954601</v>
+        <v>1270.2977134954599</v>
       </c>
       <c r="CG28">
-        <v>1286979.0355445601</v>
+        <v>1286.97903554456</v>
       </c>
       <c r="CL28">
-        <v>1296606.1476706499</v>
+        <v>1296.60614767065</v>
       </c>
     </row>
     <row r="29" spans="2:90" x14ac:dyDescent="0.25">

</xml_diff>